<commit_message>
update the boundaries for the histograms.
</commit_message>
<xml_diff>
--- a/09_calc_agb_stats/05_combine_tile_hists/gmw_v3_agb_summary_bounds.xlsx
+++ b/09_calc_agb_stats/05_combine_tile_hists/gmw_v3_agb_summary_bounds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="251">
   <si>
     <t>Country</t>
   </si>
@@ -22,22 +22,19 @@
     <t>Country_Code</t>
   </si>
   <si>
-    <t>0-250</t>
-  </si>
-  <si>
-    <t>250-500</t>
-  </si>
-  <si>
-    <t>500-750</t>
-  </si>
-  <si>
-    <t>750-1000</t>
-  </si>
-  <si>
-    <t>1000-1250</t>
-  </si>
-  <si>
-    <t>1250-</t>
+    <t>0-50</t>
+  </si>
+  <si>
+    <t>50-100</t>
+  </si>
+  <si>
+    <t>100-150</t>
+  </si>
+  <si>
+    <t>150-250</t>
+  </si>
+  <si>
+    <t>250-1500</t>
   </si>
   <si>
     <t>Angola</t>
@@ -1127,13 +1124,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1155,48 +1152,42 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2">
-        <v>0.8199442520483149</v>
+        <v>0.3710583664160824</v>
       </c>
       <c r="E2">
-        <v>0.1249531210406284</v>
+        <v>0.2324520652082102</v>
       </c>
       <c r="F2">
-        <v>0.05510262691105668</v>
+        <v>0.1148137511614157</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.1016200692626066</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>0.1800557479516851</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1213,19 +1204,16 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1242,25 +1230,22 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.8830769230769231</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.1169230769230769</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1271,19 +1256,16 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1300,83 +1282,74 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.5826696652996428</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.2639105701812409</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.07401772721259425</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.07940203730652202</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.4441556641369512</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.3533592850569667</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.2024850508060821</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.8916985441050528</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.1083014558949472</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1387,106 +1360,94 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D10">
-        <v>0.5694229062834302</v>
+        <v>0</v>
       </c>
       <c r="E10">
+        <v>0.002637100184928724</v>
+      </c>
+      <c r="F10">
+        <v>0.04541948966306484</v>
+      </c>
+      <c r="G10">
+        <v>0.5213663164354366</v>
+      </c>
+      <c r="H10">
         <v>0.4305770937165698</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.6176369458233941</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.3267385511357531</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.05562450304085273</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.7962085308056872</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.1052132701421801</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.03033175355450237</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.06824644549763033</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1503,28 +1464,25 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.9513535312799314</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.04864646872006856</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1532,141 +1490,126 @@
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15">
-        <v>0.9447121243367892</v>
+        <v>0.3535499353193723</v>
       </c>
       <c r="E15">
+        <v>0.2803014679690283</v>
+      </c>
+      <c r="F15">
+        <v>0.1959729278764131</v>
+      </c>
+      <c r="G15">
+        <v>0.1148877931719755</v>
+      </c>
+      <c r="H15">
         <v>0.05528787566321079</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16">
-        <v>0.6852655676622521</v>
+        <v>0.1198631632078947</v>
       </c>
       <c r="E16">
-        <v>0.2308512616052031</v>
+        <v>0.205513694716018</v>
       </c>
       <c r="F16">
-        <v>0.0838831707325448</v>
+        <v>0.1808216584348434</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.179067051303496</v>
       </c>
       <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>0.3147344323377479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D17">
-        <v>0.9201526475572733</v>
+        <v>0.4909594118435972</v>
       </c>
       <c r="E17">
+        <v>0.2083338413457045</v>
+      </c>
+      <c r="F17">
+        <v>0.1318515628492585</v>
+      </c>
+      <c r="G17">
+        <v>0.08900783151871314</v>
+      </c>
+      <c r="H17">
         <v>0.07984735244272669</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D18">
-        <v>0.6053215077605322</v>
+        <v>0.03288201160541586</v>
       </c>
       <c r="E18">
+        <v>0.1442185214888899</v>
+      </c>
+      <c r="F18">
+        <v>0.188281360569892</v>
+      </c>
+      <c r="G18">
+        <v>0.2399396140963344</v>
+      </c>
+      <c r="H18">
         <v>0.3946784922394678</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0.8652265992769897</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.1347734007230103</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1677,77 +1620,68 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D20">
-        <v>0.8704726826273788</v>
+        <v>0.2615101289134438</v>
       </c>
       <c r="E20">
+        <v>0.2361878453038674</v>
+      </c>
+      <c r="F20">
+        <v>0.1958256599140577</v>
+      </c>
+      <c r="G20">
+        <v>0.1769490484960098</v>
+      </c>
+      <c r="H20">
         <v>0.1295273173726212</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D21">
-        <v>0.7606786271740057</v>
+        <v>0</v>
       </c>
       <c r="E21">
+        <v>0.1191471928400088</v>
+      </c>
+      <c r="F21">
+        <v>0.2757479024621739</v>
+      </c>
+      <c r="G21">
+        <v>0.3657835318718231</v>
+      </c>
+      <c r="H21">
         <v>0.2393213728259943</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1764,86 +1698,77 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D23">
-        <v>0.6716924386606941</v>
+        <v>0</v>
       </c>
       <c r="E23">
+        <v>0.1223917080689862</v>
+      </c>
+      <c r="F23">
+        <v>0.2138285022968218</v>
+      </c>
+      <c r="G23">
+        <v>0.3354722282948861</v>
+      </c>
+      <c r="H23">
         <v>0.3283075613393059</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D24">
-        <v>0.9285914465183145</v>
+        <v>0.6302627719176604</v>
       </c>
       <c r="E24">
+        <v>0.2006162618458279</v>
+      </c>
+      <c r="F24">
+        <v>0.04421739351785632</v>
+      </c>
+      <c r="G24">
+        <v>0.05349501923696989</v>
+      </c>
+      <c r="H24">
         <v>0.07140855348168548</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0.6689853706511495</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.2322255460394214</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.09878908330942916</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1851,83 +1776,74 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1936100017364126</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.6238930369855877</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>0.1824969612779997</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0.6775544787971932</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.17942148487505</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.08407029332902956</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>0.05895374299872721</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0.9153563591838714</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>0.0846436408161286</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1938,57 +1854,51 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0.3580886586067933</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>0.4749568221070812</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>0.1105354058721934</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>0.05641911341393207</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0.7612270714737508</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.1416192283364959</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>0.09715370018975332</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1996,57 +1906,51 @@
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.334842560326459</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>0.3855774708573201</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>0.2795799688162209</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0.5220392989909719</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.3493941003234683</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>0.1285666006855598</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2054,144 +1958,129 @@
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D33">
-        <v>0.8334565163833456</v>
+        <v>0.2512934220251293</v>
       </c>
       <c r="E33">
+        <v>0.2685390490268539</v>
+      </c>
+      <c r="F33">
+        <v>0.1150529687115053</v>
+      </c>
+      <c r="G33">
+        <v>0.1985710766198571</v>
+      </c>
+      <c r="H33">
         <v>0.1665434836166544</v>
       </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D34">
-        <v>0.8992977099123463</v>
+        <v>0</v>
       </c>
       <c r="E34">
+        <v>0.08505208518663487</v>
+      </c>
+      <c r="F34">
+        <v>0.3489768663487884</v>
+      </c>
+      <c r="G34">
+        <v>0.465268758376923</v>
+      </c>
+      <c r="H34">
         <v>0.1007022900876537</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D35">
-        <v>0.8539774291219377</v>
+        <v>0.08959537572254335</v>
       </c>
       <c r="E35">
+        <v>0.2237819983484723</v>
+      </c>
+      <c r="F35">
+        <v>0.2738783374621525</v>
+      </c>
+      <c r="G35">
+        <v>0.2667217175887696</v>
+      </c>
+      <c r="H35">
         <v>0.1460225708780622</v>
       </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D36">
-        <v>0.9190682684698942</v>
+        <v>0.4359865908927416</v>
       </c>
       <c r="E36">
+        <v>0.2764092367455579</v>
+      </c>
+      <c r="F36">
+        <v>0.1267391986188044</v>
+      </c>
+      <c r="G36">
+        <v>0.07993324221279045</v>
+      </c>
+      <c r="H36">
         <v>0.08093173153010574</v>
       </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0.5818956622360191</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>0.2913643516648795</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>0.1267399860991015</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2199,106 +2088,94 @@
       <c r="H37">
         <v>0</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D38">
-        <v>0.367063492063492</v>
+        <v>0.007936507936507936</v>
       </c>
       <c r="E38">
+        <v>0.03373015873015873</v>
+      </c>
+      <c r="F38">
+        <v>0.1130952380952381</v>
+      </c>
+      <c r="G38">
+        <v>0.2123015873015873</v>
+      </c>
+      <c r="H38">
         <v>0.6329365079365079</v>
       </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D39">
-        <v>0.9164455730192782</v>
+        <v>0.3554704259883543</v>
       </c>
       <c r="E39">
+        <v>0.2469448214468135</v>
+      </c>
+      <c r="F39">
+        <v>0.1551727157304847</v>
+      </c>
+      <c r="G39">
+        <v>0.1588576098536258</v>
+      </c>
+      <c r="H39">
         <v>0.0835544269807218</v>
       </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>0.2297297297297297</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>0.558277027027027</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>0.2119932432432433</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2315,25 +2192,22 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0.8503259498107388</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>0.1496740501892612</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2344,57 +2218,51 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>0.5888888888888889</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>0.6370083816892328</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>0.3629916183107673</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2402,54 +2270,48 @@
       <c r="H44">
         <v>0</v>
       </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D45">
-        <v>0.7859045202097983</v>
+        <v>0.2237675405920298</v>
       </c>
       <c r="E45">
-        <v>0.156668605992957</v>
+        <v>0.1600786611803916</v>
       </c>
       <c r="F45">
-        <v>0.05742687379724475</v>
+        <v>0.1785312192044199</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>0.223527099232957</v>
       </c>
       <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>0.2140954797902017</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0.7956122054372303</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>0.2043877945627697</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2460,83 +2322,74 @@
       <c r="H46">
         <v>0</v>
       </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D47">
-        <v>0.9240121580547113</v>
+        <v>0.547112462006079</v>
       </c>
       <c r="E47">
+        <v>0.3009118541033435</v>
+      </c>
+      <c r="F47">
+        <v>0.0425531914893617</v>
+      </c>
+      <c r="G47">
+        <v>0.03343465045592705</v>
+      </c>
+      <c r="H47">
         <v>0.07598784194528875</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D48">
-        <v>0.7130324641869795</v>
+        <v>0.1542696801588265</v>
       </c>
       <c r="E48">
+        <v>0.1365686779612904</v>
+      </c>
+      <c r="F48">
+        <v>0.1539851171456869</v>
+      </c>
+      <c r="G48">
+        <v>0.2682089889211757</v>
+      </c>
+      <c r="H48">
         <v>0.2869675358130205</v>
       </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0.8928194993412385</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>0.1071805006587615</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2547,25 +2400,22 @@
       <c r="H49">
         <v>0</v>
       </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0.7787878787878788</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>0.2212121212121212</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2576,54 +2426,48 @@
       <c r="H50">
         <v>0</v>
       </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D51">
-        <v>0.8875673185665965</v>
+        <v>0.2624421273831614</v>
       </c>
       <c r="E51">
+        <v>0.2811192285893962</v>
+      </c>
+      <c r="F51">
+        <v>0.1735492703327303</v>
+      </c>
+      <c r="G51">
+        <v>0.1704566922613086</v>
+      </c>
+      <c r="H51">
         <v>0.1124326814334035</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0.7936799694414491</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>0.2063200305585509</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -2634,28 +2478,25 @@
       <c r="H52">
         <v>0</v>
       </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0.8411016949152542</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>0.1419491525423729</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>0.01694915254237288</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2663,106 +2504,94 @@
       <c r="H53">
         <v>0</v>
       </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D54">
-        <v>0.9450867052023122</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>0.02312138728323699</v>
+        <v>0.1589595375722543</v>
       </c>
       <c r="F54">
-        <v>0.01445086705202312</v>
+        <v>0.6820809248554913</v>
       </c>
       <c r="G54">
-        <v>0.0115606936416185</v>
+        <v>0.1040462427745665</v>
       </c>
       <c r="H54">
-        <v>0.002890173410404624</v>
-      </c>
-      <c r="I54">
-        <v>0.002890173410404624</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>0.05491329479768786</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D55">
-        <v>0.8521761861194616</v>
+        <v>0.03489739903280617</v>
       </c>
       <c r="E55">
+        <v>0.1360606456672331</v>
+      </c>
+      <c r="F55">
+        <v>0.3084564109266762</v>
+      </c>
+      <c r="G55">
+        <v>0.372761730492746</v>
+      </c>
+      <c r="H55">
         <v>0.1478238138805385</v>
       </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D56">
-        <v>0.7671051173055774</v>
+        <v>0.2029709690958933</v>
       </c>
       <c r="E56">
+        <v>0.1952352899416243</v>
+      </c>
+      <c r="F56">
+        <v>0.1480975908671409</v>
+      </c>
+      <c r="G56">
+        <v>0.2208012674009189</v>
+      </c>
+      <c r="H56">
         <v>0.2328948826944226</v>
       </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2779,54 +2608,48 @@
       <c r="H57">
         <v>0</v>
       </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>0.409590379833735</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>0.4316782951948813</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>0.1587313249713838</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0.9403166869671132</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>0.05968331303288672</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2837,25 +2660,22 @@
       <c r="H59">
         <v>0</v>
       </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0.7725888324873097</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>0.2274111675126904</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2866,199 +2686,178 @@
       <c r="H60">
         <v>0</v>
       </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D61">
-        <v>0.7571113508010513</v>
+        <v>0.1839379232702557</v>
       </c>
       <c r="E61">
+        <v>0.1808968942136089</v>
+      </c>
+      <c r="F61">
+        <v>0.1029809925421308</v>
+      </c>
+      <c r="G61">
+        <v>0.289295540775056</v>
+      </c>
+      <c r="H61">
         <v>0.2428886491989487</v>
       </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>0.0696969696969697</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>0.04747474747474748</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>0.1328282828282828</v>
       </c>
       <c r="H62">
         <v>0</v>
       </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D63">
-        <v>0.7754594369500181</v>
+        <v>0</v>
       </c>
       <c r="E63">
+        <v>0.06667178065378672</v>
+      </c>
+      <c r="F63">
+        <v>0.2628516322751033</v>
+      </c>
+      <c r="G63">
+        <v>0.4459360240211281</v>
+      </c>
+      <c r="H63">
         <v>0.2245405630499819</v>
       </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D64">
-        <v>0.7607038171413529</v>
+        <v>0.3424634696748259</v>
       </c>
       <c r="E64">
-        <v>0.1230939656756156</v>
+        <v>0.2176009125383538</v>
       </c>
       <c r="F64">
-        <v>0.0580778015722641</v>
+        <v>0.1115665881540018</v>
       </c>
       <c r="G64">
-        <v>0.0581244156107673</v>
+        <v>0.08907284677417143</v>
       </c>
       <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>0.239296182858647</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D65">
-        <v>0.8863784659166843</v>
+        <v>0.7627414447772458</v>
       </c>
       <c r="E65">
-        <v>0.05355219609600403</v>
+        <v>0.08310338592643256</v>
       </c>
       <c r="F65">
-        <v>0.06006933798731162</v>
+        <v>0.02239727050462646</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>0.01813636470837952</v>
       </c>
       <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>0.1136215340833156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0.4127913029643508</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>0.2818158367483121</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>0.1638757292710919</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>0.1415171310162452</v>
       </c>
       <c r="H66">
         <v>0</v>
       </c>
-      <c r="I66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0.6070038910505836</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>0.3929961089494163</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -3069,54 +2868,48 @@
       <c r="H67">
         <v>0</v>
       </c>
-      <c r="I67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0.3802578399803885</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>0.2922456085130336</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>0.159712256334222</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>0.1677842951723559</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0.5811965811965812</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>0.4188034188034188</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -3127,48 +2920,42 @@
       <c r="H69">
         <v>0</v>
       </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D70">
-        <v>0.9086239275324962</v>
+        <v>0.1541701955296977</v>
       </c>
       <c r="E70">
+        <v>0.1638325293662776</v>
+      </c>
+      <c r="F70">
+        <v>0.2179401259343816</v>
+      </c>
+      <c r="G70">
+        <v>0.3726810767021394</v>
+      </c>
+      <c r="H70">
         <v>0.09137607246750377</v>
       </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -3185,28 +2972,25 @@
       <c r="H71">
         <v>0</v>
       </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>0.1739130434782609</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -3214,83 +2998,74 @@
       <c r="H72">
         <v>0</v>
       </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D73">
-        <v>0.8456384252796683</v>
+        <v>0.3434569015250191</v>
       </c>
       <c r="E73">
+        <v>0.2397168796702677</v>
+      </c>
+      <c r="F73">
+        <v>0.1277867142940276</v>
+      </c>
+      <c r="G73">
+        <v>0.1346779297903539</v>
+      </c>
+      <c r="H73">
         <v>0.1543615747203317</v>
       </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D74">
-        <v>0.5034079844206426</v>
+        <v>0.02142161635832522</v>
       </c>
       <c r="E74">
-        <v>0.3485881207400195</v>
+        <v>0.1080817916260954</v>
       </c>
       <c r="F74">
-        <v>0.1480038948393379</v>
+        <v>0.1509250243427459</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>0.2229795520934761</v>
       </c>
       <c r="H74">
-        <v>0</v>
-      </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>0.4965920155793573</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0.7853914742885062</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>0.2146085257114938</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -3301,48 +3076,42 @@
       <c r="H75">
         <v>0</v>
       </c>
-      <c r="I75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C76" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0.3403531508180787</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>0.2702089745666613</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>0.2133484529402236</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>0.1760894216750364</v>
       </c>
       <c r="H76">
         <v>0</v>
       </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -3359,28 +3128,25 @@
       <c r="H77">
         <v>0</v>
       </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>0.6629788383340752</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>0.2241205979883663</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>0.1129005636775584</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3388,83 +3154,74 @@
       <c r="H78">
         <v>0</v>
       </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0.3992048070746025</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>0.2996921301385645</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>0.144026710665053</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>0.1570763521217799</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C80" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>0.4996439536476411</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>0.3325415823042547</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>0.1128379200567214</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>0.05497654399138285</v>
       </c>
       <c r="H80">
         <v>0</v>
       </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C81" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0.7658182617778022</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>0.2341817382221978</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -3475,57 +3232,51 @@
       <c r="H81">
         <v>0</v>
       </c>
-      <c r="I81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0.6270309898129102</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>0.2173358066411989</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>0.07890862229405426</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>0.07672458125183662</v>
       </c>
       <c r="H82">
         <v>0</v>
       </c>
-      <c r="I82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0.3064064203331684</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>0.4769781321930679</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>0.2166154474737637</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3533,57 +3284,51 @@
       <c r="H83">
         <v>0</v>
       </c>
-      <c r="I83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D84">
-        <v>0.8621135477840014</v>
+        <v>0.4004892611327639</v>
       </c>
       <c r="E84">
+        <v>0.2324367315245497</v>
+      </c>
+      <c r="F84">
+        <v>0.1311091678037528</v>
+      </c>
+      <c r="G84">
+        <v>0.09807838732293496</v>
+      </c>
+      <c r="H84">
         <v>0.1378864522159986</v>
       </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>0.3639558232931727</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>0.5115461847389559</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>0.1244979919678715</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -3591,86 +3336,77 @@
       <c r="H85">
         <v>0</v>
       </c>
-      <c r="I85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0.3421420840043295</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>0.3411992321414429</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>0.1658476426817724</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>0.1508110411724551</v>
       </c>
       <c r="H86">
         <v>0</v>
       </c>
-      <c r="I86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D87">
-        <v>0.7559768711193319</v>
+        <v>0.2275439990198287</v>
       </c>
       <c r="E87">
+        <v>0.1748696727887849</v>
+      </c>
+      <c r="F87">
+        <v>0.1407000320136592</v>
+      </c>
+      <c r="G87">
+        <v>0.2128631672970591</v>
+      </c>
+      <c r="H87">
         <v>0.2440231288806681</v>
       </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-      <c r="H87">
-        <v>0</v>
-      </c>
-      <c r="I87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C88" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>0.533457249070632</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>0.466542750929368</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -3678,25 +3414,22 @@
       <c r="H88">
         <v>0</v>
       </c>
-      <c r="I88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C89" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0.8974500434811068</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>0.1025499565188932</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -3707,25 +3440,22 @@
       <c r="H89">
         <v>0</v>
       </c>
-      <c r="I89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>0.9605181986428131</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>0.03948180135718692</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -3736,28 +3466,25 @@
       <c r="H90">
         <v>0</v>
       </c>
-      <c r="I90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C91" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>0.7839671366829968</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>0.2160328633170033</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -3765,57 +3492,51 @@
       <c r="H91">
         <v>0</v>
       </c>
-      <c r="I91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>0.2492620926450214</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>0.5953858201313174</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>0.1553520872236612</v>
       </c>
       <c r="H92">
         <v>0</v>
       </c>
-      <c r="I92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C93" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>0.5866437506920801</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>0.2846940732988866</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>0.1286621760090333</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3823,86 +3544,77 @@
       <c r="H93">
         <v>0</v>
       </c>
-      <c r="I93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C94" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D94">
-        <v>0.9475331039825319</v>
+        <v>0.5562210223339903</v>
       </c>
       <c r="E94">
+        <v>0.2298240684288611</v>
+      </c>
+      <c r="F94">
+        <v>0.09920818547768599</v>
+      </c>
+      <c r="G94">
+        <v>0.06227982774199452</v>
+      </c>
+      <c r="H94">
         <v>0.05246689601746813</v>
       </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>0</v>
-      </c>
-      <c r="I94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>0.4594565540758445</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>0.3404074469441479</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>0.09342179933650498</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>0.1067141996435027</v>
       </c>
       <c r="H95">
         <v>0</v>
       </c>
-      <c r="I95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>0.7337724584466183</v>
       </c>
       <c r="E96">
-        <v>0</v>
+        <v>0.1769263110687558</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>0.08930123048462595</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -3910,28 +3622,25 @@
       <c r="H96">
         <v>0</v>
       </c>
-      <c r="I96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C97" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>0.7420668183451083</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>0.1802451530029066</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>0.07768802865198507</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -3939,77 +3648,68 @@
       <c r="H97">
         <v>0</v>
       </c>
-      <c r="I97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C98" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>0.5156394598459267</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>0.3894745475760849</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>0.09488599257798838</v>
       </c>
       <c r="H98">
         <v>0</v>
       </c>
-      <c r="I98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C99" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>0.07359586830213041</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>0.7101355713363461</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>0.2162685603615236</v>
       </c>
       <c r="H99">
         <v>0</v>
       </c>
-      <c r="I99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9">
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C100" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -4026,19 +3726,16 @@
       <c r="H100">
         <v>0</v>
       </c>
-      <c r="I100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C101" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -4055,86 +3752,77 @@
       <c r="H101">
         <v>0</v>
       </c>
-      <c r="I101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C102" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D102">
-        <v>0.851260831239626</v>
+        <v>0.2174956234984784</v>
       </c>
       <c r="E102">
+        <v>0.1970164842494077</v>
+      </c>
+      <c r="F102">
+        <v>0.2142134192544064</v>
+      </c>
+      <c r="G102">
+        <v>0.2225353042373336</v>
+      </c>
+      <c r="H102">
         <v>0.148739168760374</v>
       </c>
-      <c r="F102">
-        <v>0</v>
-      </c>
-      <c r="G102">
-        <v>0</v>
-      </c>
-      <c r="H102">
-        <v>0</v>
-      </c>
-      <c r="I102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C103" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D103">
-        <v>0.9419419419419419</v>
+        <v>0.2912912912912913</v>
       </c>
       <c r="E103">
+        <v>0.3143143143143143</v>
+      </c>
+      <c r="F103">
+        <v>0.1301301301301301</v>
+      </c>
+      <c r="G103">
+        <v>0.2062062062062062</v>
+      </c>
+      <c r="H103">
         <v>0.05805805805805806</v>
       </c>
-      <c r="F103">
-        <v>0</v>
-      </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-      <c r="H103">
-        <v>0</v>
-      </c>
-      <c r="I103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9">
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C104" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>0.7949691111734095</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>0.1347894657828425</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>0.070241423043748</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4142,57 +3830,51 @@
       <c r="H104">
         <v>0</v>
       </c>
-      <c r="I104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C105" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>0.05232558139534884</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>0.5494186046511628</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>0.3982558139534884</v>
       </c>
       <c r="H105">
         <v>0</v>
       </c>
-      <c r="I105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C106" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>0.8041778490680467</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>0.1958221509319534</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4200,25 +3882,22 @@
       <c r="H106">
         <v>0</v>
       </c>
-      <c r="I106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C107" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0.6823599753124517</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>0.3176400246875482</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -4229,106 +3908,94 @@
       <c r="H107">
         <v>0</v>
       </c>
-      <c r="I107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C108" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>0.5462912171412202</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>0.3535307502159433</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>0.1001780326428365</v>
       </c>
       <c r="H108">
         <v>0</v>
       </c>
-      <c r="I108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" s="1">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C109" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D109">
-        <v>0.8219862690987413</v>
+        <v>0</v>
       </c>
       <c r="E109">
+        <v>0.006915931883960422</v>
+      </c>
+      <c r="F109">
+        <v>0.3075654573601669</v>
+      </c>
+      <c r="G109">
+        <v>0.507504879854614</v>
+      </c>
+      <c r="H109">
         <v>0.1780137309012587</v>
       </c>
-      <c r="F109">
-        <v>0</v>
-      </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
-      <c r="I109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" s="1">
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C110" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D110">
-        <v>0.5807476254095615</v>
+        <v>0</v>
       </c>
       <c r="E110">
+        <v>0.04370238894300513</v>
+      </c>
+      <c r="F110">
+        <v>0.11060973382085</v>
+      </c>
+      <c r="G110">
+        <v>0.4264355026457063</v>
+      </c>
+      <c r="H110">
         <v>0.4192523745904385</v>
       </c>
-      <c r="F110">
-        <v>0</v>
-      </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" s="1">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C111" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -4345,48 +4012,42 @@
       <c r="H111">
         <v>0</v>
       </c>
-      <c r="I111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" s="1">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C112" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D112">
-        <v>0.860204335908298</v>
+        <v>0.1996012957886868</v>
       </c>
       <c r="E112">
+        <v>0.1898828806379267</v>
+      </c>
+      <c r="F112">
+        <v>0.2162970346374284</v>
+      </c>
+      <c r="G112">
+        <v>0.2544231248442562</v>
+      </c>
+      <c r="H112">
         <v>0.139795664091702</v>
       </c>
-      <c r="F112">
-        <v>0</v>
-      </c>
-      <c r="G112">
-        <v>0</v>
-      </c>
-      <c r="H112">
-        <v>0</v>
-      </c>
-      <c r="I112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" s="1">
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C113" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -4403,83 +4064,74 @@
       <c r="H113">
         <v>0</v>
       </c>
-      <c r="I113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114" s="1">
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C114" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>0.46875</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>0.3984375</v>
       </c>
       <c r="G114">
-        <v>0</v>
+        <v>0.1328125</v>
       </c>
       <c r="H114">
         <v>0</v>
       </c>
-      <c r="I114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C115" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D115">
-        <v>0.9278516727126159</v>
+        <v>0</v>
       </c>
       <c r="E115">
+        <v>0.0592503022974607</v>
+      </c>
+      <c r="F115">
+        <v>0.6400644901249496</v>
+      </c>
+      <c r="G115">
+        <v>0.2285368802902056</v>
+      </c>
+      <c r="H115">
         <v>0.07214832728738411</v>
       </c>
-      <c r="F115">
-        <v>0</v>
-      </c>
-      <c r="G115">
-        <v>0</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
-      <c r="I115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116" s="1">
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C116" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0.8946078431372549</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>0.1053921568627451</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -4490,86 +4142,77 @@
       <c r="H116">
         <v>0</v>
       </c>
-      <c r="I116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117" s="1">
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C117" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>0.2527632711310335</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>0.6171544150424726</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>0.130082313826494</v>
       </c>
       <c r="H117">
         <v>0</v>
       </c>
-      <c r="I117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" s="1">
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C118" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D118">
-        <v>0.8450080135759405</v>
+        <v>0</v>
       </c>
       <c r="E118">
+        <v>0.3466578674460262</v>
+      </c>
+      <c r="F118">
+        <v>0.2741585745262562</v>
+      </c>
+      <c r="G118">
+        <v>0.224191571603658</v>
+      </c>
+      <c r="H118">
         <v>0.1549919864240596</v>
       </c>
-      <c r="F118">
-        <v>0</v>
-      </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
-      <c r="H118">
-        <v>0</v>
-      </c>
-      <c r="I118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" s="1">
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C119" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>0.6992026395380808</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>0.3007973604619192</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -4577,54 +4220,48 @@
       <c r="H119">
         <v>0</v>
       </c>
-      <c r="I119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C120" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>0.2811247326656304</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>0.3836525763436839</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>0.2232519546086692</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>0.1119707363820164</v>
       </c>
       <c r="H120">
         <v>0</v>
       </c>
-      <c r="I120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C121" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0.9382022471910112</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>0.06179775280898876</v>
       </c>
       <c r="F121">
         <v>0</v>
@@ -4635,25 +4272,22 @@
       <c r="H121">
         <v>0</v>
       </c>
-      <c r="I121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C122" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0.8886763580719205</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>0.1113236419280796</v>
       </c>
       <c r="F122">
         <v>0</v>
@@ -4664,37 +4298,31 @@
       <c r="H122">
         <v>0</v>
       </c>
-      <c r="I122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C123" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D123">
-        <v>0.8044534280963714</v>
+        <v>0.4181201708342842</v>
       </c>
       <c r="E123">
-        <v>0.1020767450200502</v>
+        <v>0.1877221008704724</v>
       </c>
       <c r="F123">
-        <v>0.0934698268835784</v>
+        <v>0.09940338408372185</v>
       </c>
       <c r="G123">
-        <v>0</v>
+        <v>0.09920777230789293</v>
       </c>
       <c r="H123">
-        <v>0</v>
-      </c>
-      <c r="I123">
-        <v>0</v>
+        <v>0.1955465719036286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>